<commit_message>
Escaleta 2 con DBA
Se incluyeron los Derechos Básicos de Aprendizaje
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/ESCALETA_LE_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/ESCALETA_LE_06_02_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado06\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA\NUEVO\ESCALETAS\Escaletas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7698"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -384,9 +384,6 @@
     <t>En este recurso se busca que los estudiantes se acerquen a los textos narrativos y a sus principales características</t>
   </si>
   <si>
-    <t>La idea es poner varios fragmentos de textos narrativos para que los estudiantes identifiquen en ellos, entre otros: temáticas, estructura (inicio, nudo, final), personajes, tiempo, espacios, ideas principales, ideas secundarias, etc.</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>El estudiante podrá clasificar distintos textos según pertenezcan al sentido figurado o al sentido propio</t>
   </si>
   <si>
-    <t xml:space="preserve">Se deben escoger frases o textos que sirvan claramente de ejemplos sobre el uso figurado y el uso propio o estricto del lenguaje para que el estudiante los clasifique dentro de los contenedores respectivos.  </t>
-  </si>
-  <si>
     <t>Recurso M10A-01</t>
   </si>
   <si>
@@ -417,9 +411,6 @@
     <t>En esta actividad el estudiante debe ser capaz de identificar en un texto dado las expresiones que tienen algún sentido figurado</t>
   </si>
   <si>
-    <t>Se busca presentar un texto al estudiante en el que haya ejemplos de usos figurados del lenguaje y ejemplos de sentido propio. La actividad podría consistir en que el estudiante identifique solo aquellos que considere de sentido figurado. Se podría pensar en usar un texto de tipo narrativo.</t>
-  </si>
-  <si>
     <t>Recurso M13B-01</t>
   </si>
   <si>
@@ -444,9 +435,6 @@
     <t>El estudiante podrá escuchar y clasificar los textos que escucha en algunos géneros informativos como el reportaje, la entrevista o la noticia</t>
   </si>
   <si>
-    <t xml:space="preserve">La idea es incluir ejemplos de audios de una noticia, de una entrevista y de un reportaje a fin de que el estudiante logre escucharlos y clasificarlos. </t>
-  </si>
-  <si>
     <t>Recurso M3B-01</t>
   </si>
   <si>
@@ -462,15 +450,9 @@
     <t>Lo ideal sería poner varios ejemplos de expresiones orales y hacerle preguntas a los estudiantes en las que identifiquen los usos que se hace de la lengua de acuerdo a lo escuchado. Por ejemplo, puede haber un audio en el que se utilice la función apelativa del lenguaje y se le pregunte al estudiante por ello.</t>
   </si>
   <si>
-    <t>Cömo podemos clasificar los textos literarios</t>
-  </si>
-  <si>
     <t>SÍ</t>
   </si>
   <si>
-    <t xml:space="preserve">Hay que hacer una selección de textos literarios pertenecientes a los distintos géneros: narrativo, lírico y dramático. Se le pueden plantear preguntas a los estudiantes para hacerles evidentes las diferencias entre los textos presentados y el porqué de su clasificación. </t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -528,9 +510,6 @@
     <t>Actividad para que el estudiante identifique características del género narrativo</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_01_REC280). La idea es plantear un ejercicio de creación narrativa.</t>
-  </si>
-  <si>
     <t>Reforcemos nuestro aprendizaje sobre el género dramático</t>
   </si>
   <si>
@@ -564,9 +543,6 @@
     <t>Sí</t>
   </si>
   <si>
-    <t xml:space="preserve">Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC40). Hay que revisar que el contenido sea preciso y con un lenguaje adecuado. </t>
-  </si>
-  <si>
     <t>Recurso expositivo que acerca al estudiante a comprender los elementos literarios que trabajan con el sentido figurado</t>
   </si>
   <si>
@@ -579,10 +555,6 @@
     <t>Actividad para aprender a diferenciar oraciones escritas en sentido propio o en sentido figurado</t>
   </si>
   <si>
-    <t xml:space="preserve">Hay que recordar la adaptación hecha por el autor (LE_06_07_REC60). Él sugiere "Cambiar la frase costar diez euros por costar diez mil pesos" y dejar el resto de texto del recurso igual.
-</t>
-  </si>
-  <si>
     <t>El poema</t>
   </si>
   <si>
@@ -595,9 +567,6 @@
     <t>Actividad que motiva al estudiante a identificar el sentido correcto de las expresiones figurativas</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC30). Hay que tener en cuenta que cambia el título y la descripción (se sigue la de la escaleta).</t>
-  </si>
-  <si>
     <t>Recurso M1C-01</t>
   </si>
   <si>
@@ -637,9 +606,6 @@
     <t>Explora algunos géneros informativos y comunicativos</t>
   </si>
   <si>
-    <t>Recurso nuevo. En este recurso se deben presentar algunas características generales de las noticias, los reportajes y las entrevistas. Cada uno puede estar representado en alguna imagen. Se puede aprovechar la información que no se tenga en cuenta para el recurso 37 de la primera escaleta que tiene que ver con guión.</t>
-  </si>
-  <si>
     <t>Recurso F6-02</t>
   </si>
   <si>
@@ -652,27 +618,18 @@
     <t>Interactivo para analizar el contenido y la estructura básica de una noticia; además permite diferenciar entre noticia escrita y noticia gráfica</t>
   </si>
   <si>
-    <t>Hay que utilizar el recurso introduciendo los cambios que sugirió la autora al adaptar el recurso (ver la tabla correspondiente LE_06_11_REC20 en el archivo LE_06_11).</t>
-  </si>
-  <si>
     <t>Los géneros informativos: la noticia escrita y la noticia gráfica</t>
   </si>
   <si>
     <t>Actividad para practicar la identificación de las partes de la noticia</t>
   </si>
   <si>
-    <t>El recurso queda igual salvo por el título</t>
-  </si>
-  <si>
     <t>Identifica las partes de una noticia</t>
   </si>
   <si>
     <t>Actividad para acercar a los estudiantes al formato de la entrevista de manera práctica</t>
   </si>
   <si>
-    <t xml:space="preserve">Recurso nuevo. Hay que plantear una actividad en la que los estudiantes se organicen para presentar un pequeño noticiero. Para ello, primero deben redactar las noticias y luego escoger la mejor manera para poderlas comunicar, con organización. Ya que este recurso permite adjuntar archivos, lo ideal sería que le presentáramos al estudiante una pequeña plantilla que puede utilizar a la hora de escribir noticias. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC50). </t>
   </si>
   <si>
@@ -700,9 +657,6 @@
     <t>Recurso para organizar las características necesarias en la redacción de un reportaje</t>
   </si>
   <si>
-    <t>Recurso nuevo. La idea es identificar algunas características esenciales para la redacción de un reportaje (por ejemplo, la estructura, la intención comunicativa, el uso del lenguaje) y plantear un ejercicio de contenedores, en el que el estudiante deba organizar y clasificar dichas características.</t>
-  </si>
-  <si>
     <t>Recurso M10A-02</t>
   </si>
   <si>
@@ -712,9 +666,6 @@
     <t>Actividad para que los estudiantes aborden el reconocimiento de textos informativos</t>
   </si>
   <si>
-    <t xml:space="preserve">Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC70). </t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -826,9 +777,6 @@
     <t>Actividad para escuchar diversos textos, reconocer sus características y realizar su clasificación</t>
   </si>
   <si>
-    <t>Recurso nuevo. La idea es realizar algunos audios de distintos textos pertenecientes a los géneros literarios para que le estudiante al escucharlos pueda clasificarlos.</t>
-  </si>
-  <si>
     <t>Recurso M3B-02</t>
   </si>
   <si>
@@ -844,9 +792,6 @@
     <t>Recurso M12A-01</t>
   </si>
   <si>
-    <t>Es un recurso completamente nuevo. Se debe buscar una buena selección de textos de los diferentes géneros literarios. La idea es que el estudiante pueda identificar en ellos algunas características que permitan clasificarlos en un determinado género literario.</t>
-  </si>
-  <si>
     <t>Recurso nuevo. En este recurso se deben plantear algunas características de los noticieros y brindar el espacio para que el estudiante escriba en qué consisten.</t>
   </si>
   <si>
@@ -856,12 +801,6 @@
     <t xml:space="preserve">recurso para que el estudiante brinde ejemplos o explique las características del sentido figurado y del sentido propio </t>
   </si>
   <si>
-    <t>La idea es plantear algunas preguntas para que el estudiante brinde ejemplos sobre el sentido figurado y el sentido propio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Este recurso es nuevo pero podemos aprovechar la información del recurso elaborado por el autor anteriormente (LE_06_07_REC80). </t>
-  </si>
-  <si>
     <t>Recurso M101A-07</t>
   </si>
   <si>
@@ -907,9 +846,6 @@
     <t xml:space="preserve">Interactivo para que el estudiante aborde el proceso de escritura a partir del desarrollo de un plan textual </t>
   </si>
   <si>
-    <t>La idea es presentar un plan textual estructurado para que el estudiante desarrolle fases en su propio escrito. Lo ideal sería que fuera con un tipo de texto relacionado con los géneros literarios (se debe plantear una actividad de escritura en la que sea claramente identificable la intención comunicativa).</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proyecto: el proceso de escritura con un plan textual </t>
   </si>
   <si>
@@ -917,6 +853,69 @@
   </si>
   <si>
     <t>RM_01_02_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cömo podemos clasificar los textos literarios </t>
+  </si>
+  <si>
+    <t>Es un recurso completamente nuevo. Se debe buscar una buena selección de textos de los diferentes géneros literarios. La idea es que el estudiante pueda identificar en ellos algunas características que permitan clasificarlos en un determinado género literario. DBA1</t>
+  </si>
+  <si>
+    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC40). Hay que revisar que el contenido sea preciso y con un lenguaje adecuado. DBA1</t>
+  </si>
+  <si>
+    <t>La idea es presentar un plan textual estructurado para que el estudiante desarrolle fases en su propio escrito. Lo ideal sería que fuera con un tipo de texto relacionado con los géneros literarios (se debe plantear una actividad de escritura en la que sea claramente identificable la intención comunicativa). DBA2</t>
+  </si>
+  <si>
+    <t>El recurso queda igual salvo por el título. DBA1 - DBA6</t>
+  </si>
+  <si>
+    <t>Recurso nuevo. La idea es identificar algunas características esenciales para la redacción de un reportaje (por ejemplo, la estructura, la intención comunicativa, el uso del lenguaje) y plantear un ejercicio de contenedores, en el que el estudiante deba organizar y clasificar dichas características. DBA6</t>
+  </si>
+  <si>
+    <t>Se busca presentar un texto al estudiante en el que haya ejemplos de usos figurados del lenguaje y ejemplos de sentido propio. La actividad podría consistir en que el estudiante identifique solo aquellos que considere de sentido figurado. Se podría pensar en usar un texto de tipo narrativo. DBA 8</t>
+  </si>
+  <si>
+    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC30). Hay que tener en cuenta que cambia el título y la descripción (se sigue la de la escaleta). DBA8</t>
+  </si>
+  <si>
+    <t>Hay que recordar la adaptación hecha por el autor (LE_06_07_REC60). Él sugiere "Cambiar la frase costar diez euros por costar diez mil pesos" y dejar el resto de texto del recurso igual. DBA8</t>
+  </si>
+  <si>
+    <t>La idea es plantear algunas preguntas para que el estudiante brinde ejemplos sobre el sentido figurado y el sentido propio. DBA8</t>
+  </si>
+  <si>
+    <t>Hay que hacer una selección de textos literarios pertenecientes a los distintos géneros: narrativo, lírico y dramático. Se le pueden plantear preguntas a los estudiantes para hacerles evidentes las diferencias entre los textos presentados y el porqué de su clasificación. DBA1 - DBA9</t>
+  </si>
+  <si>
+    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_01_REC280). La idea es plantear un ejercicio de creación narrativa. DBA9</t>
+  </si>
+  <si>
+    <t>Recurso nuevo. La idea es realizar algunos audios de distintos textos pertenecientes a los géneros literarios para que le estudiante al escucharlos pueda clasificarlos. DBA9</t>
+  </si>
+  <si>
+    <t>Recurso nuevo. En este recurso se deben presentar algunas características generales de las noticias, los reportajes y las entrevistas. Cada uno puede estar representado en alguna imagen. Se puede aprovechar la información que no se tenga en cuenta para el recurso 37 de la primera escaleta que tiene que ver con guión. DBA10</t>
+  </si>
+  <si>
+    <t>Hay que utilizar el recurso introduciendo los cambios que sugirió la autora al adaptar el recurso (ver la tabla correspondiente LE_06_11_REC20 en el archivo LE_06_11). DBA10</t>
+  </si>
+  <si>
+    <t>Recurso elaborado por el autor. Aprobado para digitalizar. Usar y aprovechar el recurso que se había planteado anteriormente (LE_06_07_REC70). DBA10</t>
+  </si>
+  <si>
+    <t>Este recurso es nuevo pero podemos aprovechar la información del recurso elaborado por el autor anteriormente (LE_06_07_REC80). DBA1 - DBA10</t>
+  </si>
+  <si>
+    <t>Recurso nuevo. Hay que plantear una actividad en la que los estudiantes se organicen para presentar un pequeño noticiero. Para ello, primero deben redactar las noticias y luego escoger la mejor manera para poderlas comunicar, con organización. Ya que este recurso permite adjuntar archivos, lo ideal sería que le presentáramos al estudiante una pequeña plantilla que puede utilizar a la hora de escribir noticias. DBA2 - DBA4 - DBA11</t>
+  </si>
+  <si>
+    <t>Se deben escoger frases o textos que sirvan claramente de ejemplos sobre el uso figurado y el uso propio o estricto del lenguaje para que el estudiante los clasifique dentro de los contenedores respectivos. DBA8</t>
+  </si>
+  <si>
+    <t>La idea es poner varios fragmentos de textos narrativos para que los estudiantes identifiquen en ellos, entre otros: temáticas, estructura (inicio, nudo, final), personajes, tiempo, espacios, ideas principales, ideas secundarias, etc. DBA6</t>
+  </si>
+  <si>
+    <t>La idea es incluir ejemplos de audios de una noticia, de una entrevista y de un reportaje a fin de que el estudiante logre escucharlos y clasificarlos. DBA10</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1376,6 +1375,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1676,127 +1678,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.46484375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="27.796875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="17.46484375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="21.265625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="46.73046875" style="17" customWidth="1"/>
-    <col min="8" max="8" width="4.9296875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="42.73046875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="8.1328125" style="48" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="48" customWidth="1"/>
-    <col min="13" max="13" width="7.53125" style="17" customWidth="1"/>
-    <col min="14" max="14" width="7.53125" style="48" customWidth="1"/>
-    <col min="15" max="15" width="21.59765625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="42.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="48" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="48" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" style="48" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" style="17" customWidth="1"/>
     <col min="16" max="16" width="8" style="2" customWidth="1"/>
-    <col min="17" max="17" width="6.59765625" style="17" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="17" customWidth="1"/>
     <col min="18" max="18" width="10" style="17" customWidth="1"/>
-    <col min="19" max="19" width="26.73046875" style="17" customWidth="1"/>
-    <col min="20" max="20" width="25.6640625" style="17" customWidth="1"/>
-    <col min="21" max="21" width="13.73046875" style="17" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="17"/>
+    <col min="19" max="19" width="26.7109375" style="17" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" style="17" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="17" customWidth="1"/>
+    <col min="22" max="16384" width="10.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="49" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="Q1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="54"/>
+    <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="55"/>
       <c r="M2" s="16" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
@@ -1812,7 +1814,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -1834,7 +1836,7 @@
         <v>84</v>
       </c>
       <c r="O3" s="25" t="s">
-        <v>119</v>
+        <v>295</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>19</v>
@@ -1843,19 +1845,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="U3" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>68</v>
       </c>
@@ -1871,7 +1873,7 @@
       <c r="E4" s="28"/>
       <c r="F4" s="21"/>
       <c r="G4" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H4" s="11">
         <v>2</v>
@@ -1880,7 +1882,7 @@
         <v>117</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>69</v>
@@ -1893,7 +1895,7 @@
         <v>24</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>126</v>
+        <v>294</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>19</v>
@@ -1902,19 +1904,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S4" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T4" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U4" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>68</v>
       </c>
@@ -1930,7 +1932,7 @@
       <c r="E5" s="28"/>
       <c r="F5" s="21"/>
       <c r="G5" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="11">
         <v>3</v>
@@ -1939,7 +1941,7 @@
         <v>117</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K5" s="24" t="s">
         <v>69</v>
@@ -1952,7 +1954,7 @@
         <v>59</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>130</v>
+        <v>282</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>19</v>
@@ -1961,19 +1963,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T5" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="U5" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
@@ -1989,7 +1991,7 @@
       <c r="E6" s="28"/>
       <c r="F6" s="21"/>
       <c r="G6" s="22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H6" s="11">
         <v>4</v>
@@ -1998,7 +2000,7 @@
         <v>117</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K6" s="24" t="s">
         <v>69</v>
@@ -2011,7 +2013,7 @@
         <v>82</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P6" s="13" t="s">
         <v>19</v>
@@ -2020,19 +2022,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S6" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S6" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T6" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="U6" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>68</v>
       </c>
@@ -2048,7 +2050,7 @@
       <c r="E7" s="28"/>
       <c r="F7" s="21"/>
       <c r="G7" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H7" s="11">
         <v>5</v>
@@ -2057,7 +2059,7 @@
         <v>117</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K7" s="24" t="s">
         <v>69</v>
@@ -2070,7 +2072,7 @@
         <v>79</v>
       </c>
       <c r="O7" s="25" t="s">
-        <v>139</v>
+        <v>296</v>
       </c>
       <c r="P7" s="13" t="s">
         <v>19</v>
@@ -2079,19 +2081,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S7" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T7" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="U7" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>68</v>
       </c>
@@ -2107,7 +2109,7 @@
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
       <c r="G8" s="22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H8" s="11">
         <v>6</v>
@@ -2116,7 +2118,7 @@
         <v>117</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K8" s="24" t="s">
         <v>69</v>
@@ -2129,7 +2131,7 @@
         <v>83</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P8" s="13" t="s">
         <v>19</v>
@@ -2138,19 +2140,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S8" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T8" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U8" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>68</v>
       </c>
@@ -2166,16 +2168,16 @@
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
       <c r="G9" s="22" t="s">
-        <v>145</v>
+        <v>276</v>
       </c>
       <c r="H9" s="12">
         <v>7</v>
       </c>
       <c r="I9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="32" t="s">
         <v>146</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>152</v>
       </c>
       <c r="K9" s="33" t="s">
         <v>69</v>
@@ -2188,7 +2190,7 @@
       </c>
       <c r="N9" s="25"/>
       <c r="O9" s="34" t="s">
-        <v>147</v>
+        <v>286</v>
       </c>
       <c r="P9" s="13" t="s">
         <v>19</v>
@@ -2197,19 +2199,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="U9" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>68</v>
       </c>
@@ -2227,16 +2229,16 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="22" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H10" s="12">
         <v>8</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K10" s="33" t="s">
         <v>70</v>
@@ -2247,28 +2249,28 @@
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="34" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P10" s="13" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="R10" s="26" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S10" s="26" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="T10" s="26" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="U10" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>68</v>
       </c>
@@ -2288,7 +2290,7 @@
         <v>99</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H11" s="12">
         <v>9</v>
@@ -2297,7 +2299,7 @@
         <v>117</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="K11" s="33" t="s">
         <v>69</v>
@@ -2310,7 +2312,7 @@
         <v>62</v>
       </c>
       <c r="O11" s="34" t="s">
-        <v>167</v>
+        <v>287</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>19</v>
@@ -2319,19 +2321,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S11" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S11" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T11" s="8" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="U11" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>68</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>100</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H12" s="12">
         <v>10</v>
@@ -2360,7 +2362,7 @@
         <v>117</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="K12" s="33" t="s">
         <v>69</v>
@@ -2373,7 +2375,7 @@
         <v>62</v>
       </c>
       <c r="O12" s="34" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="P12" s="13" t="s">
         <v>19</v>
@@ -2382,19 +2384,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S12" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T12" s="8" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="U12" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>68</v>
       </c>
@@ -2414,7 +2416,7 @@
         <v>101</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H13" s="12">
         <v>11</v>
@@ -2423,7 +2425,7 @@
         <v>117</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="K13" s="33" t="s">
         <v>69</v>
@@ -2436,7 +2438,7 @@
         <v>62</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="P13" s="13" t="s">
         <v>19</v>
@@ -2445,19 +2447,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S13" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S13" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T13" s="8" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="U13" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>68</v>
       </c>
@@ -2475,7 +2477,7 @@
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="35" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H14" s="12">
         <v>12</v>
@@ -2484,7 +2486,7 @@
         <v>117</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="K14" s="33" t="s">
         <v>70</v>
@@ -2495,28 +2497,28 @@
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="34" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="P14" s="13" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="U14" s="37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>68</v>
       </c>
@@ -2534,7 +2536,7 @@
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="35" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H15" s="12">
         <v>13</v>
@@ -2543,7 +2545,7 @@
         <v>117</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K15" s="33" t="s">
         <v>69</v>
@@ -2556,7 +2558,7 @@
         <v>62</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="P15" s="13" t="s">
         <v>20</v>
@@ -2565,19 +2567,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S15" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S15" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T15" s="8" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="U15" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>68</v>
       </c>
@@ -2595,7 +2597,7 @@
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="35" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H16" s="12">
         <v>14</v>
@@ -2604,7 +2606,7 @@
         <v>117</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="K16" s="33" t="s">
         <v>69</v>
@@ -2617,7 +2619,7 @@
         <v>73</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="P16" s="13" t="s">
         <v>19</v>
@@ -2626,19 +2628,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S16" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S16" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T16" s="8" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="U16" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>68</v>
       </c>
@@ -2656,7 +2658,7 @@
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="35" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H17" s="12">
         <v>15</v>
@@ -2665,7 +2667,7 @@
         <v>117</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="K17" s="33" t="s">
         <v>69</v>
@@ -2678,7 +2680,7 @@
         <v>74</v>
       </c>
       <c r="O17" s="34" t="s">
-        <v>189</v>
+        <v>283</v>
       </c>
       <c r="P17" s="13" t="s">
         <v>19</v>
@@ -2687,19 +2689,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S17" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S17" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T17" s="8" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="U17" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>68</v>
       </c>
@@ -2717,16 +2719,16 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="35" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H18" s="12">
         <v>16</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="K18" s="33" t="s">
         <v>69</v>
@@ -2739,7 +2741,7 @@
       </c>
       <c r="N18" s="25"/>
       <c r="O18" s="34" t="s">
-        <v>179</v>
+        <v>278</v>
       </c>
       <c r="P18" s="13" t="s">
         <v>19</v>
@@ -2748,19 +2750,19 @@
         <v>6</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="U18" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>68</v>
       </c>
@@ -2778,7 +2780,7 @@
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H19" s="12">
         <v>17</v>
@@ -2787,7 +2789,7 @@
         <v>117</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K19" s="33" t="s">
         <v>70</v>
@@ -2797,8 +2799,8 @@
       </c>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="34" t="s">
-        <v>184</v>
+      <c r="O19" s="49" t="s">
+        <v>284</v>
       </c>
       <c r="P19" s="13" t="s">
         <v>19</v>
@@ -2807,19 +2809,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="U19" s="37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>68</v>
       </c>
@@ -2837,7 +2839,7 @@
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="35" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="H20" s="12">
         <v>18</v>
@@ -2846,7 +2848,7 @@
         <v>117</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="K20" s="33" t="s">
         <v>69</v>
@@ -2859,7 +2861,7 @@
         <v>62</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="P20" s="13" t="s">
         <v>19</v>
@@ -2868,19 +2870,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S20" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S20" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T20" s="8" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="U20" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>68</v>
       </c>
@@ -2898,16 +2900,16 @@
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="35" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H21" s="12">
         <v>19</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="K21" s="33" t="s">
         <v>69</v>
@@ -2920,7 +2922,7 @@
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="34" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="P21" s="13" t="s">
         <v>19</v>
@@ -2929,19 +2931,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="U21" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>68</v>
       </c>
@@ -2959,7 +2961,7 @@
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="35" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="H22" s="12">
         <v>20</v>
@@ -2968,7 +2970,7 @@
         <v>117</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="K22" s="33" t="s">
         <v>69</v>
@@ -2981,7 +2983,7 @@
         <v>64</v>
       </c>
       <c r="O22" s="34" t="s">
-        <v>214</v>
+        <v>293</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>19</v>
@@ -2990,19 +2992,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S22" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S22" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T22" s="8" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="U22" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>68</v>
       </c>
@@ -3020,7 +3022,7 @@
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="35" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H23" s="12">
         <v>21</v>
@@ -3029,7 +3031,7 @@
         <v>117</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="K23" s="33" t="s">
         <v>69</v>
@@ -3042,7 +3044,7 @@
         <v>62</v>
       </c>
       <c r="O23" s="34" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>19</v>
@@ -3051,19 +3053,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S23" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T23" s="8" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="U23" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>68</v>
       </c>
@@ -3081,7 +3083,7 @@
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="35" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="H24" s="12">
         <v>22</v>
@@ -3090,7 +3092,7 @@
         <v>117</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="K24" s="33" t="s">
         <v>69</v>
@@ -3103,7 +3105,7 @@
         <v>74</v>
       </c>
       <c r="O24" s="34" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>20</v>
@@ -3112,19 +3114,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S24" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S24" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T24" s="8" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="U24" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>68</v>
       </c>
@@ -3140,16 +3142,16 @@
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
       <c r="G25" s="35" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H25" s="12">
         <v>23</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="K25" s="33" t="s">
         <v>69</v>
@@ -3162,7 +3164,7 @@
       </c>
       <c r="N25" s="25"/>
       <c r="O25" s="34" t="s">
-        <v>203</v>
+        <v>289</v>
       </c>
       <c r="P25" s="13" t="s">
         <v>19</v>
@@ -3171,19 +3173,19 @@
         <v>6</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="U25" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>68</v>
       </c>
@@ -3201,16 +3203,16 @@
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="35" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H26" s="12">
         <v>24</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J26" s="32" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="K26" s="33" t="s">
         <v>70</v>
@@ -3221,7 +3223,7 @@
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
       <c r="O26" s="34" t="s">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="P26" s="13" t="s">
         <v>19</v>
@@ -3230,19 +3232,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S26" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="U26" s="37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>68</v>
       </c>
@@ -3260,7 +3262,7 @@
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="35" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="H27" s="12">
         <v>25</v>
@@ -3269,7 +3271,7 @@
         <v>117</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K27" s="33" t="s">
         <v>70</v>
@@ -3280,7 +3282,7 @@
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="34" t="s">
-        <v>211</v>
+        <v>280</v>
       </c>
       <c r="P27" s="13" t="s">
         <v>19</v>
@@ -3289,19 +3291,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="U27" s="37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>68</v>
       </c>
@@ -3319,7 +3321,7 @@
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="35" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="H28" s="12">
         <v>26</v>
@@ -3328,7 +3330,7 @@
         <v>117</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="K28" s="33" t="s">
         <v>69</v>
@@ -3341,7 +3343,7 @@
         <v>24</v>
       </c>
       <c r="O28" s="34" t="s">
-        <v>224</v>
+        <v>281</v>
       </c>
       <c r="P28" s="13" t="s">
         <v>19</v>
@@ -3350,19 +3352,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S28" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S28" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T28" s="8" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="U28" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>68</v>
       </c>
@@ -3380,7 +3382,7 @@
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="35" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H29" s="12">
         <v>27</v>
@@ -3389,7 +3391,7 @@
         <v>117</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="K29" s="33" t="s">
         <v>69</v>
@@ -3402,7 +3404,7 @@
         <v>62</v>
       </c>
       <c r="O29" s="34" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="P29" s="13" t="s">
         <v>19</v>
@@ -3411,19 +3413,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S29" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S29" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T29" s="8" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="U29" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>68</v>
       </c>
@@ -3441,7 +3443,7 @@
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="35" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="H30" s="12">
         <v>28</v>
@@ -3450,7 +3452,7 @@
         <v>117</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="K30" s="33" t="s">
         <v>69</v>
@@ -3463,7 +3465,7 @@
         <v>23</v>
       </c>
       <c r="O30" s="34" t="s">
-        <v>228</v>
+        <v>291</v>
       </c>
       <c r="P30" s="13" t="s">
         <v>20</v>
@@ -3472,19 +3474,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S30" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S30" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T30" s="8" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="U30" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>68</v>
       </c>
@@ -3502,7 +3504,7 @@
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="35" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="H31" s="12">
         <v>29</v>
@@ -3511,7 +3513,7 @@
         <v>117</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="K31" s="33" t="s">
         <v>69</v>
@@ -3524,7 +3526,7 @@
         <v>62</v>
       </c>
       <c r="O31" s="34" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="P31" s="13" t="s">
         <v>19</v>
@@ -3533,19 +3535,19 @@
         <v>6</v>
       </c>
       <c r="R31" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S31" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S31" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T31" s="8" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="U31" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>68</v>
       </c>
@@ -3556,21 +3558,21 @@
         <v>95</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="29"/>
       <c r="G32" s="32" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="H32" s="12">
         <v>30</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="K32" s="33" t="s">
         <v>69</v>
@@ -3583,7 +3585,7 @@
       </c>
       <c r="N32" s="25"/>
       <c r="O32" s="34" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="P32" s="13" t="s">
         <v>19</v>
@@ -3592,19 +3594,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S32" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T32" s="8" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="U32" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>68</v>
       </c>
@@ -3615,14 +3617,14 @@
         <v>95</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>113</v>
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="35" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="H33" s="12">
         <v>31</v>
@@ -3631,7 +3633,7 @@
         <v>117</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="K33" s="33" t="s">
         <v>69</v>
@@ -3644,7 +3646,7 @@
         <v>24</v>
       </c>
       <c r="O33" s="34" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="P33" s="13" t="s">
         <v>19</v>
@@ -3653,19 +3655,19 @@
         <v>6</v>
       </c>
       <c r="R33" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S33" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S33" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T33" s="8" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="U33" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>68</v>
       </c>
@@ -3676,14 +3678,14 @@
         <v>95</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E34" s="40" t="s">
         <v>114</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="35" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H34" s="12">
         <v>32</v>
@@ -3692,7 +3694,7 @@
         <v>117</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="K34" s="33" t="s">
         <v>69</v>
@@ -3705,7 +3707,7 @@
         <v>83</v>
       </c>
       <c r="O34" s="34" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="P34" s="13" t="s">
         <v>19</v>
@@ -3714,19 +3716,19 @@
         <v>6</v>
       </c>
       <c r="R34" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S34" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S34" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T34" s="8" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="U34" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>68</v>
       </c>
@@ -3737,14 +3739,14 @@
         <v>95</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E35" s="40" t="s">
         <v>115</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="35" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="H35" s="12">
         <v>33</v>
@@ -3753,7 +3755,7 @@
         <v>117</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="K35" s="33" t="s">
         <v>69</v>
@@ -3766,7 +3768,7 @@
         <v>62</v>
       </c>
       <c r="O35" s="34" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="P35" s="13" t="s">
         <v>19</v>
@@ -3775,19 +3777,19 @@
         <v>6</v>
       </c>
       <c r="R35" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S35" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S35" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T35" s="8" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="U35" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>68</v>
       </c>
@@ -3798,14 +3800,14 @@
         <v>95</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>91</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="35" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="H36" s="12">
         <v>34</v>
@@ -3814,7 +3816,7 @@
         <v>117</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="K36" s="33" t="s">
         <v>69</v>
@@ -3827,7 +3829,7 @@
         <v>53</v>
       </c>
       <c r="O36" s="34" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="P36" s="13" t="s">
         <v>20</v>
@@ -3836,19 +3838,19 @@
         <v>6</v>
       </c>
       <c r="R36" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S36" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S36" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T36" s="8" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="U36" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>68</v>
       </c>
@@ -3859,14 +3861,14 @@
         <v>95</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E37" s="40" t="s">
         <v>91</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="35" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="H37" s="12">
         <v>35</v>
@@ -3875,7 +3877,7 @@
         <v>117</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="K37" s="33" t="s">
         <v>69</v>
@@ -3888,7 +3890,7 @@
         <v>62</v>
       </c>
       <c r="O37" s="34" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="P37" s="13" t="s">
         <v>19</v>
@@ -3897,19 +3899,19 @@
         <v>6</v>
       </c>
       <c r="R37" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S37" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S37" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T37" s="8" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="U37" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>68</v>
       </c>
@@ -3925,7 +3927,7 @@
       <c r="E38" s="40"/>
       <c r="F38" s="29"/>
       <c r="G38" s="35" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="H38" s="12">
         <v>36</v>
@@ -3934,7 +3936,7 @@
         <v>117</v>
       </c>
       <c r="J38" s="32" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="K38" s="33" t="s">
         <v>69</v>
@@ -3947,7 +3949,7 @@
         <v>79</v>
       </c>
       <c r="O38" s="34" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="P38" s="13" t="s">
         <v>19</v>
@@ -3956,19 +3958,19 @@
         <v>6</v>
       </c>
       <c r="R38" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S38" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S38" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T38" s="8" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="U38" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>68</v>
       </c>
@@ -3984,7 +3986,7 @@
       <c r="E39" s="40"/>
       <c r="F39" s="29"/>
       <c r="G39" s="35" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="H39" s="12">
         <v>37</v>
@@ -3993,7 +3995,7 @@
         <v>117</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="K39" s="33" t="s">
         <v>69</v>
@@ -4006,7 +4008,7 @@
         <v>54</v>
       </c>
       <c r="O39" s="34" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="P39" s="13" t="s">
         <v>19</v>
@@ -4015,19 +4017,19 @@
         <v>6</v>
       </c>
       <c r="R39" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S39" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S39" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T39" s="8" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="U39" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>68</v>
       </c>
@@ -4043,7 +4045,7 @@
       <c r="E40" s="40"/>
       <c r="F40" s="29"/>
       <c r="G40" s="35" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="H40" s="12">
         <v>38</v>
@@ -4052,7 +4054,7 @@
         <v>117</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="K40" s="33" t="s">
         <v>69</v>
@@ -4065,7 +4067,7 @@
         <v>74</v>
       </c>
       <c r="O40" s="34" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="P40" s="13" t="s">
         <v>19</v>
@@ -4074,19 +4076,19 @@
         <v>6</v>
       </c>
       <c r="R40" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S40" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S40" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T40" s="8" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="U40" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>68</v>
       </c>
@@ -4102,7 +4104,7 @@
       <c r="E41" s="40"/>
       <c r="F41" s="29"/>
       <c r="G41" s="35" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="H41" s="12">
         <v>39</v>
@@ -4111,7 +4113,7 @@
         <v>117</v>
       </c>
       <c r="J41" s="32" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="K41" s="33" t="s">
         <v>69</v>
@@ -4124,7 +4126,7 @@
         <v>64</v>
       </c>
       <c r="O41" s="34" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="P41" s="13" t="s">
         <v>19</v>
@@ -4133,19 +4135,19 @@
         <v>6</v>
       </c>
       <c r="R41" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S41" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="S41" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="T41" s="8" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="U41" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>68</v>
       </c>
@@ -4156,12 +4158,12 @@
         <v>95</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="29"/>
       <c r="G42" s="35" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="H42" s="12">
         <v>40</v>
@@ -4170,7 +4172,7 @@
         <v>117</v>
       </c>
       <c r="J42" s="32" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="K42" s="33" t="s">
         <v>69</v>
@@ -4188,7 +4190,7 @@
       <c r="T42" s="7"/>
       <c r="U42" s="37"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>68</v>
       </c>
@@ -4199,7 +4201,7 @@
         <v>95</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="29"/>
@@ -4213,7 +4215,7 @@
         <v>117</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="K43" s="33" t="s">
         <v>69</v>
@@ -4231,19 +4233,19 @@
         <v>6</v>
       </c>
       <c r="R43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="S43" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="S43" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="T43" s="7" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="U43" s="37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>68</v>
       </c>
@@ -4254,7 +4256,7 @@
         <v>95</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="29"/>
@@ -4266,7 +4268,7 @@
         <v>117</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="K44" s="33" t="s">
         <v>69</v>
@@ -4279,7 +4281,7 @@
         <v>63</v>
       </c>
       <c r="O44" s="34" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="P44" s="13" t="s">
         <v>20</v>
@@ -4288,19 +4290,19 @@
         <v>6</v>
       </c>
       <c r="R44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="S44" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="S44" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="T44" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="U44" s="37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
@@ -4323,7 +4325,7 @@
       <c r="T45" s="7"/>
       <c r="U45" s="37"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="41"/>
       <c r="C46" s="42"/>
@@ -4346,7 +4348,7 @@
       <c r="T46" s="7"/>
       <c r="U46" s="37"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="41"/>
       <c r="C47" s="42"/>
@@ -4369,7 +4371,7 @@
       <c r="T47" s="7"/>
       <c r="U47" s="37"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="41"/>
       <c r="C48" s="42"/>
@@ -4392,7 +4394,7 @@
       <c r="T48" s="7"/>
       <c r="U48" s="37"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="30"/>
       <c r="B49" s="41"/>
       <c r="C49" s="42"/>
@@ -4415,7 +4417,7 @@
       <c r="T49" s="7"/>
       <c r="U49" s="37"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="41"/>
       <c r="C50" s="42"/>
@@ -4438,7 +4440,7 @@
       <c r="T50" s="7"/>
       <c r="U50" s="37"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="41"/>
       <c r="C51" s="42"/>
@@ -4461,7 +4463,7 @@
       <c r="T51" s="7"/>
       <c r="U51" s="37"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="30"/>
       <c r="B52" s="41"/>
       <c r="C52" s="42"/>
@@ -4484,7 +4486,7 @@
       <c r="T52" s="7"/>
       <c r="U52" s="37"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" s="41"/>
       <c r="C53" s="42"/>
@@ -4507,7 +4509,7 @@
       <c r="T53" s="7"/>
       <c r="U53" s="37"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="30"/>
       <c r="B54" s="41"/>
       <c r="C54" s="42"/>
@@ -4530,7 +4532,7 @@
       <c r="T54" s="7"/>
       <c r="U54" s="37"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
       <c r="B55" s="41"/>
       <c r="C55" s="42"/>
@@ -4553,7 +4555,7 @@
       <c r="T55" s="7"/>
       <c r="U55" s="37"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="41"/>
       <c r="C56" s="42"/>
@@ -4576,7 +4578,7 @@
       <c r="T56" s="7"/>
       <c r="U56" s="37"/>
     </row>
-    <row r="57" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="41"/>
       <c r="C57" s="42"/>
@@ -4599,7 +4601,7 @@
       <c r="T57" s="7"/>
       <c r="U57" s="37"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" s="41"/>
       <c r="C58" s="42"/>
@@ -4622,7 +4624,7 @@
       <c r="T58" s="7"/>
       <c r="U58" s="37"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" s="41"/>
       <c r="C59" s="42"/>
@@ -4645,7 +4647,7 @@
       <c r="T59" s="7"/>
       <c r="U59" s="37"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" s="41"/>
       <c r="C60" s="42"/>
@@ -4668,7 +4670,7 @@
       <c r="T60" s="7"/>
       <c r="U60" s="37"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
       <c r="B61" s="41"/>
       <c r="C61" s="42"/>
@@ -4691,7 +4693,7 @@
       <c r="T61" s="7"/>
       <c r="U61" s="37"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
       <c r="B62" s="41"/>
       <c r="C62" s="42"/>
@@ -4714,7 +4716,7 @@
       <c r="T62" s="7"/>
       <c r="U62" s="37"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
       <c r="B63" s="41"/>
       <c r="C63" s="42"/>
@@ -4737,7 +4739,7 @@
       <c r="T63" s="7"/>
       <c r="U63" s="37"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
       <c r="B64" s="41"/>
       <c r="C64" s="42"/>
@@ -4760,7 +4762,7 @@
       <c r="T64" s="7"/>
       <c r="U64" s="37"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="30"/>
       <c r="B65" s="41"/>
       <c r="C65" s="42"/>
@@ -4783,7 +4785,7 @@
       <c r="T65" s="7"/>
       <c r="U65" s="37"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="30"/>
       <c r="B66" s="41"/>
       <c r="C66" s="42"/>
@@ -4806,7 +4808,7 @@
       <c r="T66" s="7"/>
       <c r="U66" s="37"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="30"/>
       <c r="B67" s="41"/>
       <c r="C67" s="42"/>
@@ -4829,7 +4831,7 @@
       <c r="T67" s="7"/>
       <c r="U67" s="37"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="30"/>
       <c r="B68" s="41"/>
       <c r="C68" s="42"/>
@@ -4852,7 +4854,7 @@
       <c r="T68" s="7"/>
       <c r="U68" s="37"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="30"/>
       <c r="B69" s="41"/>
       <c r="C69" s="42"/>
@@ -4875,7 +4877,7 @@
       <c r="T69" s="7"/>
       <c r="U69" s="37"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="30"/>
       <c r="B70" s="41"/>
       <c r="C70" s="42"/>
@@ -4898,7 +4900,7 @@
       <c r="T70" s="7"/>
       <c r="U70" s="37"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="30"/>
       <c r="B71" s="41"/>
       <c r="C71" s="42"/>
@@ -4921,7 +4923,7 @@
       <c r="T71" s="7"/>
       <c r="U71" s="37"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="30"/>
       <c r="B72" s="41"/>
       <c r="C72" s="42"/>
@@ -4944,7 +4946,7 @@
       <c r="T72" s="7"/>
       <c r="U72" s="37"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="30"/>
       <c r="B73" s="41"/>
       <c r="C73" s="42"/>
@@ -4967,7 +4969,7 @@
       <c r="T73" s="7"/>
       <c r="U73" s="37"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="30"/>
       <c r="B74" s="41"/>
       <c r="C74" s="42"/>
@@ -4990,7 +4992,7 @@
       <c r="T74" s="7"/>
       <c r="U74" s="37"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="30"/>
       <c r="B75" s="41"/>
       <c r="C75" s="42"/>
@@ -5013,7 +5015,7 @@
       <c r="T75" s="7"/>
       <c r="U75" s="37"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="30"/>
       <c r="B76" s="41"/>
       <c r="C76" s="42"/>
@@ -5036,7 +5038,7 @@
       <c r="T76" s="7"/>
       <c r="U76" s="37"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="30"/>
       <c r="B77" s="41"/>
       <c r="C77" s="42"/>
@@ -5059,7 +5061,7 @@
       <c r="T77" s="7"/>
       <c r="U77" s="37"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="30"/>
       <c r="B78" s="41"/>
       <c r="C78" s="42"/>
@@ -5082,7 +5084,7 @@
       <c r="T78" s="7"/>
       <c r="U78" s="37"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="30"/>
       <c r="B79" s="41"/>
       <c r="C79" s="42"/>
@@ -5105,7 +5107,7 @@
       <c r="T79" s="7"/>
       <c r="U79" s="37"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="30"/>
       <c r="B80" s="41"/>
       <c r="C80" s="42"/>
@@ -5128,7 +5130,7 @@
       <c r="T80" s="7"/>
       <c r="U80" s="37"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="30"/>
       <c r="B81" s="41"/>
       <c r="C81" s="42"/>
@@ -5151,7 +5153,7 @@
       <c r="T81" s="7"/>
       <c r="U81" s="37"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="30"/>
       <c r="B82" s="41"/>
       <c r="C82" s="42"/>
@@ -5174,7 +5176,7 @@
       <c r="T82" s="7"/>
       <c r="U82" s="37"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="30"/>
       <c r="B83" s="41"/>
       <c r="C83" s="42"/>
@@ -5197,7 +5199,7 @@
       <c r="T83" s="7"/>
       <c r="U83" s="37"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="30"/>
       <c r="B84" s="41"/>
       <c r="C84" s="42"/>
@@ -5220,7 +5222,7 @@
       <c r="T84" s="7"/>
       <c r="U84" s="37"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="30"/>
       <c r="B85" s="41"/>
       <c r="C85" s="42"/>
@@ -5243,7 +5245,7 @@
       <c r="T85" s="7"/>
       <c r="U85" s="37"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="30"/>
       <c r="B86" s="41"/>
       <c r="C86" s="42"/>
@@ -5266,7 +5268,7 @@
       <c r="T86" s="7"/>
       <c r="U86" s="37"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="30"/>
       <c r="B87" s="41"/>
       <c r="C87" s="42"/>
@@ -5289,7 +5291,7 @@
       <c r="T87" s="7"/>
       <c r="U87" s="37"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="30"/>
       <c r="B88" s="41"/>
       <c r="C88" s="42"/>
@@ -5312,7 +5314,7 @@
       <c r="T88" s="7"/>
       <c r="U88" s="37"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="30"/>
       <c r="B89" s="41"/>
       <c r="C89" s="42"/>
@@ -5335,7 +5337,7 @@
       <c r="T89" s="7"/>
       <c r="U89" s="37"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="30"/>
       <c r="B90" s="41"/>
       <c r="C90" s="42"/>
@@ -5358,7 +5360,7 @@
       <c r="T90" s="7"/>
       <c r="U90" s="37"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="30"/>
       <c r="B91" s="41"/>
       <c r="C91" s="42"/>
@@ -5381,7 +5383,7 @@
       <c r="T91" s="7"/>
       <c r="U91" s="37"/>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="30"/>
       <c r="B92" s="41"/>
       <c r="C92" s="42"/>
@@ -5404,7 +5406,7 @@
       <c r="T92" s="7"/>
       <c r="U92" s="37"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="30"/>
       <c r="B93" s="41"/>
       <c r="C93" s="42"/>
@@ -5427,7 +5429,7 @@
       <c r="T93" s="7"/>
       <c r="U93" s="37"/>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="30"/>
       <c r="B94" s="41"/>
       <c r="C94" s="42"/>
@@ -5450,7 +5452,7 @@
       <c r="T94" s="7"/>
       <c r="U94" s="37"/>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="30"/>
       <c r="B95" s="41"/>
       <c r="C95" s="42"/>
@@ -5473,7 +5475,7 @@
       <c r="T95" s="7"/>
       <c r="U95" s="37"/>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="30"/>
       <c r="B96" s="41"/>
       <c r="C96" s="42"/>
@@ -5496,7 +5498,7 @@
       <c r="T96" s="7"/>
       <c r="U96" s="37"/>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="30"/>
       <c r="B97" s="41"/>
       <c r="C97" s="42"/>
@@ -5519,7 +5521,7 @@
       <c r="T97" s="7"/>
       <c r="U97" s="37"/>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="30"/>
       <c r="B98" s="41"/>
       <c r="C98" s="42"/>
@@ -5542,7 +5544,7 @@
       <c r="T98" s="7"/>
       <c r="U98" s="37"/>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="30"/>
       <c r="B99" s="41"/>
       <c r="C99" s="42"/>
@@ -5565,7 +5567,7 @@
       <c r="T99" s="7"/>
       <c r="U99" s="37"/>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="30"/>
       <c r="B100" s="41"/>
       <c r="C100" s="42"/>
@@ -5588,7 +5590,7 @@
       <c r="T100" s="7"/>
       <c r="U100" s="37"/>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="30"/>
       <c r="B101" s="41"/>
       <c r="C101" s="42"/>
@@ -5611,7 +5613,7 @@
       <c r="T101" s="7"/>
       <c r="U101" s="37"/>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="30"/>
       <c r="B102" s="41"/>
       <c r="C102" s="42"/>
@@ -5634,7 +5636,7 @@
       <c r="T102" s="7"/>
       <c r="U102" s="37"/>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="30"/>
       <c r="B103" s="41"/>
       <c r="C103" s="42"/>
@@ -5657,7 +5659,7 @@
       <c r="T103" s="7"/>
       <c r="U103" s="37"/>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="30"/>
       <c r="B104" s="41"/>
       <c r="C104" s="42"/>
@@ -5680,7 +5682,7 @@
       <c r="T104" s="7"/>
       <c r="U104" s="37"/>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="30"/>
       <c r="B105" s="41"/>
       <c r="C105" s="42"/>
@@ -5703,7 +5705,7 @@
       <c r="T105" s="7"/>
       <c r="U105" s="37"/>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="30"/>
       <c r="B106" s="41"/>
       <c r="C106" s="42"/>
@@ -5804,16 +5806,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
@@ -5836,7 +5838,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
         <v>34</v>
@@ -5857,7 +5859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>35</v>
@@ -5878,7 +5880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
         <v>36</v>
@@ -5895,7 +5897,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
         <v>37</v>
@@ -5912,7 +5914,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>38</v>
@@ -5927,7 +5929,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>39</v>
@@ -5940,7 +5942,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>40</v>
@@ -5953,7 +5955,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9" t="s">
         <v>41</v>
@@ -5966,7 +5968,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
         <v>42</v>
@@ -5979,7 +5981,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>43</v>
@@ -5994,7 +5996,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
         <v>44</v>
@@ -6009,7 +6011,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>45</v>
@@ -6024,7 +6026,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>46</v>
@@ -6039,7 +6041,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
@@ -6052,7 +6054,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
@@ -6065,7 +6067,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
@@ -6078,7 +6080,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
@@ -6091,7 +6093,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
@@ -6104,7 +6106,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9" t="s">
@@ -6117,7 +6119,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
@@ -6130,7 +6132,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9" t="s">
@@ -6143,7 +6145,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9" t="s">
@@ -6156,7 +6158,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
@@ -6169,7 +6171,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
@@ -6180,7 +6182,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9" t="s">
@@ -6191,7 +6193,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9" t="s">
@@ -6202,7 +6204,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9" t="s">
@@ -6213,7 +6215,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9" t="s">
@@ -6224,7 +6226,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9" t="s">
@@ -6235,7 +6237,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
@@ -6246,7 +6248,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9" t="s">
@@ -6257,7 +6259,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9" t="s">
@@ -6268,7 +6270,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9" t="s">
@@ -6279,7 +6281,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
@@ -6290,7 +6292,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
@@ -6301,7 +6303,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="9" t="s">
@@ -6312,7 +6314,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
@@ -6323,7 +6325,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
@@ -6334,7 +6336,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -6343,7 +6345,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -6352,7 +6354,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -6361,7 +6363,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -6370,7 +6372,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -6379,7 +6381,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -6388,7 +6390,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -6397,7 +6399,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -6406,7 +6408,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -6415,7 +6417,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -6424,7 +6426,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>

</xml_diff>